<commit_message>
discussed with developers about test cases, and executed them
</commit_message>
<xml_diff>
--- a/apps/features/backlog/android/devices/connected_device.xlsx
+++ b/apps/features/backlog/android/devices/connected_device.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\office\SymlexVPNTestCases\apps\features\backlog\android\devices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DA3BFF-8563-4B01-B815-0936C0F6A4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BCA78D-E1C1-428D-8561-31162B436345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="95">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -412,9 +412,6 @@
   </si>
   <si>
     <t xml:space="preserve">should be same </t>
-  </si>
-  <si>
-    <t>SYM-WIN-CD-022</t>
   </si>
 </sst>
 </file>
@@ -1273,7 +1270,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G32" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G31" dataDxfId="7">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID" dataDxfId="6"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites" dataDxfId="5"/>
@@ -1492,7 +1489,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2450,24 +2447,12 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="121.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>87</v>
-      </c>
+      <c r="A25" s="12"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="7"/>
       <c r="G25" s="18"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
@@ -2548,9 +2533,9 @@
     <row r="28" spans="1:26" ht="96" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12"/>
       <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
+      <c r="C28" s="12"/>
       <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
+      <c r="E28" s="12"/>
       <c r="F28" s="7"/>
       <c r="G28" s="18"/>
       <c r="H28" s="1"/>
@@ -2631,11 +2616,11 @@
     </row>
     <row r="31" spans="1:26" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="12"/>
-      <c r="B31" s="9"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="12"/>
-      <c r="D31" s="9"/>
+      <c r="D31" s="12"/>
       <c r="E31" s="12"/>
-      <c r="F31" s="7"/>
+      <c r="F31" s="18"/>
       <c r="G31" s="18"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
@@ -2658,13 +2643,13 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" ht="80.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="12"/>
-      <c r="B32" s="12"/>
-      <c r="C32" s="12"/>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="18"/>
-      <c r="G32" s="18"/>
+      <c r="A32" s="10"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="10"/>
+      <c r="E32" s="13"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
@@ -2687,7 +2672,7 @@
     </row>
     <row r="33" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
-      <c r="B33" s="9"/>
+      <c r="B33" s="10"/>
       <c r="C33" s="13"/>
       <c r="D33" s="10"/>
       <c r="E33" s="13"/>
@@ -29482,13 +29467,6 @@
       <c r="Z989" s="1"/>
     </row>
     <row r="990" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A990" s="10"/>
-      <c r="B990" s="10"/>
-      <c r="C990" s="13"/>
-      <c r="D990" s="10"/>
-      <c r="E990" s="13"/>
-      <c r="F990" s="5"/>
-      <c r="G990" s="5"/>
       <c r="H990" s="1"/>
       <c r="I990" s="1"/>
       <c r="J990" s="1"/>
@@ -29514,7 +29492,7 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F32" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F31" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>